<commit_message>
Add TCR test data, update test docs
</commit_message>
<xml_diff>
--- a/test/sequencing_layout/Sequencing_Layout_template.xlsx
+++ b/test/sequencing_layout/Sequencing_Layout_template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4A7D6D-1FF6-47DB-9F2F-DEC26E681E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="652"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample input" sheetId="1" r:id="rId1"/>
@@ -15,11 +21,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sample input'!$A$1:$E$97</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'printable layout'!$A$2:$M$15</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
@@ -30,7 +33,11 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -645,8 +652,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="41" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1882,25 +1889,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="57" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="57" customWidth="1"/>
+    <col min="1" max="1" width="16.41015625" style="57" customWidth="1"/>
+    <col min="2" max="2" width="16.29296875" style="57" customWidth="1"/>
     <col min="3" max="3" width="34" style="117" customWidth="1"/>
     <col min="4" max="4" width="14" style="119" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="57" customWidth="1"/>
+    <col min="5" max="5" width="32.703125" style="57" customWidth="1"/>
     <col min="6" max="6" width="11" style="57"/>
-    <col min="7" max="7" width="18.28515625" style="57" customWidth="1"/>
-    <col min="8" max="8" width="39.140625" style="115" customWidth="1"/>
+    <col min="7" max="7" width="18.29296875" style="57" customWidth="1"/>
+    <col min="8" max="8" width="39.1171875" style="115" customWidth="1"/>
     <col min="9" max="9" width="11" style="87"/>
-    <col min="10" max="10" width="27.28515625" style="87" customWidth="1"/>
+    <col min="10" max="10" width="27.29296875" style="87" customWidth="1"/>
     <col min="11" max="11" width="11" style="87"/>
     <col min="12" max="16384" width="11" style="57"/>
   </cols>
@@ -1932,15 +1939,15 @@
       <c r="B2" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>8</v>
+      <c r="D2" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="E2" s="88" t="str">
         <f>CONCATENATE(C2,"+",D2)</f>
-        <v>sample1+NEF1F</v>
+        <v>sample1+GS1R</v>
       </c>
       <c r="M2" s="87"/>
       <c r="N2" s="87"/>
@@ -1952,35 +1959,35 @@
       <c r="B3" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>8</v>
+      <c r="D3" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="E3" s="88" t="str">
         <f t="shared" ref="E3:E66" si="0">CONCATENATE(C3,"+",D3)</f>
-        <v>sample2+NEF1F</v>
+        <v>sample2+GA783F</v>
       </c>
       <c r="M3" s="87"/>
       <c r="N3" s="87"/>
     </row>
-    <row r="4" spans="1:14" ht="15">
+    <row r="4" spans="1:14">
       <c r="A4" s="86">
         <v>3</v>
       </c>
       <c r="B4" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="132" t="s">
+      <c r="C4" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>8</v>
+      <c r="D4" s="10" t="s">
+        <v>2</v>
       </c>
       <c r="E4" s="88" t="str">
         <f t="shared" si="0"/>
-        <v>sample3+NEF1F</v>
+        <v>sample3+GAS4R</v>
       </c>
       <c r="M4" s="87"/>
       <c r="N4" s="87"/>
@@ -1992,15 +1999,15 @@
       <c r="B5" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>8</v>
+      <c r="D5" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="E5" s="88" t="str">
         <f t="shared" si="0"/>
-        <v>sample4+NEF1F</v>
+        <v>sample4+GAS6R</v>
       </c>
       <c r="M5" s="87"/>
       <c r="N5" s="87"/>
@@ -2012,35 +2019,35 @@
       <c r="B6" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="D6" s="41" t="s">
-        <v>8</v>
+      <c r="D6" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="E6" s="88" t="str">
         <f t="shared" si="0"/>
-        <v>sample5+NEF1F</v>
+        <v>sample5+HPR2027R</v>
       </c>
       <c r="M6" s="87"/>
       <c r="N6" s="87"/>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14">
       <c r="A7" s="86">
         <v>6</v>
       </c>
       <c r="B7" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="D7" s="41" t="s">
-        <v>8</v>
+      <c r="D7" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E7" s="88" t="str">
         <f t="shared" si="0"/>
-        <v>sample6+NEF1F</v>
+        <v>sample6+HPR1977F</v>
       </c>
       <c r="L7" s="87"/>
       <c r="M7" s="87"/>
@@ -2053,15 +2060,15 @@
       <c r="B8" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="D8" s="41" t="s">
-        <v>8</v>
+      <c r="D8" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="E8" s="88" t="str">
         <f t="shared" si="0"/>
-        <v>sample7+NEF1F</v>
+        <v>sample7+GS3F</v>
       </c>
       <c r="L8" s="87"/>
       <c r="M8" s="87"/>
@@ -2074,15 +2081,15 @@
       <c r="B9" s="90" t="s">
         <v>99</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="D9" s="41" t="s">
-        <v>8</v>
+      <c r="D9" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="E9" s="88" t="str">
         <f t="shared" si="0"/>
-        <v>sample8+NEF1F</v>
+        <v>sample8+GS5F</v>
       </c>
       <c r="L9" s="87"/>
       <c r="M9" s="87"/>
@@ -2443,7 +2450,7 @@
       <c r="M29" s="87"/>
       <c r="N29" s="87"/>
     </row>
-    <row r="30" spans="1:14" ht="17">
+    <row r="30" spans="1:14" ht="18">
       <c r="A30" s="86">
         <v>29</v>
       </c>
@@ -2691,7 +2698,7 @@
       <c r="H45" s="111"/>
       <c r="I45" s="120"/>
     </row>
-    <row r="46" spans="1:9" ht="17">
+    <row r="46" spans="1:9" ht="18">
       <c r="A46" s="86">
         <v>45</v>
       </c>
@@ -3552,7 +3559,7 @@
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3563,8 +3570,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:M14"/>
@@ -3573,14 +3580,14 @@
       <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.65"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="14" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.87890625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.1171875" customWidth="1"/>
+    <col min="3" max="3" width="29.87890625" customWidth="1"/>
+    <col min="4" max="4" width="32.87890625" customWidth="1"/>
+    <col min="5" max="5" width="28.41015625" customWidth="1"/>
+    <col min="6" max="14" width="25.703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -3647,7 +3654,7 @@
       </c>
       <c r="B7" s="2" t="str">
         <f>'sample input'!E2</f>
-        <v>sample1+NEF1F</v>
+        <v>sample1+GS1R</v>
       </c>
       <c r="C7" s="2" t="str">
         <f>'sample input'!E10</f>
@@ -3700,7 +3707,7 @@
       </c>
       <c r="B8" s="2" t="str">
         <f>'sample input'!E3</f>
-        <v>sample2+NEF1F</v>
+        <v>sample2+GA783F</v>
       </c>
       <c r="C8" s="2" t="str">
         <f>'sample input'!E11</f>
@@ -3753,7 +3760,7 @@
       </c>
       <c r="B9" s="2" t="str">
         <f>'sample input'!E4</f>
-        <v>sample3+NEF1F</v>
+        <v>sample3+GAS4R</v>
       </c>
       <c r="C9" s="2" t="str">
         <f>'sample input'!E12</f>
@@ -3806,7 +3813,7 @@
       </c>
       <c r="B10" s="2" t="str">
         <f>'sample input'!E5</f>
-        <v>sample4+NEF1F</v>
+        <v>sample4+GAS6R</v>
       </c>
       <c r="C10" s="2" t="str">
         <f>'sample input'!E13</f>
@@ -3859,7 +3866,7 @@
       </c>
       <c r="B11" s="2" t="str">
         <f>'sample input'!E6</f>
-        <v>sample5+NEF1F</v>
+        <v>sample5+HPR2027R</v>
       </c>
       <c r="C11" s="2" t="str">
         <f>'sample input'!E14</f>
@@ -3912,7 +3919,7 @@
       </c>
       <c r="B12" s="2" t="str">
         <f>'sample input'!E7</f>
-        <v>sample6+NEF1F</v>
+        <v>sample6+HPR1977F</v>
       </c>
       <c r="C12" s="2" t="str">
         <f>'sample input'!E15</f>
@@ -3965,7 +3972,7 @@
       </c>
       <c r="B13" s="2" t="str">
         <f>'sample input'!E8</f>
-        <v>sample7+NEF1F</v>
+        <v>sample7+GS3F</v>
       </c>
       <c r="C13" s="2" t="str">
         <f>'sample input'!E16</f>
@@ -4018,7 +4025,7 @@
       </c>
       <c r="B14" s="2" t="str">
         <f>'sample input'!E9</f>
-        <v>sample8+NEF1F</v>
+        <v>sample8+GS5F</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>'sample input'!E17</f>
@@ -4079,33 +4086,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AT32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D9" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4"/>
   <cols>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.87890625" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="52" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" style="11" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" customWidth="1"/>
-    <col min="23" max="23" width="27.85546875" customWidth="1"/>
-    <col min="24" max="24" width="21.28515625" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" customWidth="1"/>
-    <col min="26" max="26" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.41015625" customWidth="1"/>
+    <col min="13" max="13" width="5.703125" customWidth="1"/>
+    <col min="16" max="16" width="17.29296875" style="52" customWidth="1"/>
+    <col min="19" max="19" width="15.703125" style="11" customWidth="1"/>
+    <col min="21" max="21" width="15.41015625" customWidth="1"/>
+    <col min="22" max="22" width="16.29296875" customWidth="1"/>
+    <col min="23" max="23" width="27.87890625" customWidth="1"/>
+    <col min="24" max="24" width="21.29296875" customWidth="1"/>
+    <col min="25" max="25" width="14.41015625" customWidth="1"/>
+    <col min="26" max="26" width="24.29296875" customWidth="1"/>
     <col min="29" max="29" width="15" customWidth="1"/>
-    <col min="30" max="30" width="25.28515625" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" style="110" customWidth="1"/>
-    <col min="32" max="32" width="25.28515625" customWidth="1"/>
-    <col min="33" max="33" width="19.140625" customWidth="1"/>
-    <col min="34" max="34" width="16.140625" customWidth="1"/>
+    <col min="30" max="30" width="25.29296875" customWidth="1"/>
+    <col min="31" max="31" width="14.703125" style="110" customWidth="1"/>
+    <col min="32" max="32" width="25.29296875" customWidth="1"/>
+    <col min="33" max="33" width="19.1171875" customWidth="1"/>
+    <col min="34" max="34" width="16.1171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -4160,7 +4167,7 @@
       <c r="AH1" s="71"/>
       <c r="AJ1" s="71"/>
     </row>
-    <row r="2" spans="1:46" ht="17">
+    <row r="2" spans="1:46" ht="18.399999999999999">
       <c r="A2" s="10" t="s">
         <v>67</v>
       </c>
@@ -4224,7 +4231,7 @@
       <c r="AS2" s="118"/>
       <c r="AT2" s="118"/>
     </row>
-    <row r="3" spans="1:46" ht="17">
+    <row r="3" spans="1:46" ht="18">
       <c r="A3" s="10" t="s">
         <v>68</v>
       </c>
@@ -4281,7 +4288,7 @@
       <c r="AN3" s="118"/>
       <c r="AO3" s="118"/>
     </row>
-    <row r="4" spans="1:46" ht="17">
+    <row r="4" spans="1:46" ht="18">
       <c r="A4" s="10" t="s">
         <v>69</v>
       </c>
@@ -4337,7 +4344,7 @@
       <c r="AN4" s="118"/>
       <c r="AO4" s="118"/>
     </row>
-    <row r="5" spans="1:46" ht="17">
+    <row r="5" spans="1:46" ht="18.399999999999999">
       <c r="A5" s="10" t="s">
         <v>70</v>
       </c>
@@ -4393,7 +4400,7 @@
       <c r="AN5" s="118"/>
       <c r="AO5" s="118"/>
     </row>
-    <row r="6" spans="1:46" ht="17">
+    <row r="6" spans="1:46" ht="18.399999999999999">
       <c r="A6" s="10" t="s">
         <v>71</v>
       </c>
@@ -4449,7 +4456,7 @@
       <c r="AN6" s="118"/>
       <c r="AO6" s="118"/>
     </row>
-    <row r="7" spans="1:46" ht="17">
+    <row r="7" spans="1:46" ht="18.399999999999999">
       <c r="A7" s="12" t="s">
         <v>72</v>
       </c>
@@ -4506,7 +4513,7 @@
       <c r="AN7" s="118"/>
       <c r="AO7" s="118"/>
     </row>
-    <row r="8" spans="1:46" ht="17">
+    <row r="8" spans="1:46" ht="18.399999999999999">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -4548,7 +4555,7 @@
       <c r="AN8" s="118"/>
       <c r="AO8" s="118"/>
     </row>
-    <row r="9" spans="1:46" ht="17">
+    <row r="9" spans="1:46" ht="18.399999999999999">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -4590,7 +4597,7 @@
       <c r="AN9" s="118"/>
       <c r="AO9" s="118"/>
     </row>
-    <row r="10" spans="1:46" ht="17">
+    <row r="10" spans="1:46" ht="18.399999999999999">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -4627,7 +4634,7 @@
       <c r="AN10" s="118"/>
       <c r="AO10" s="118"/>
     </row>
-    <row r="11" spans="1:46" ht="17">
+    <row r="11" spans="1:46" ht="18">
       <c r="E11" s="100"/>
       <c r="F11" s="126"/>
       <c r="J11" s="25"/>
@@ -4657,7 +4664,7 @@
       <c r="AN11" s="118"/>
       <c r="AO11" s="118"/>
     </row>
-    <row r="12" spans="1:46" ht="17">
+    <row r="12" spans="1:46" ht="18">
       <c r="E12" s="120" t="s">
         <v>180</v>
       </c>
@@ -4689,7 +4696,7 @@
       <c r="AN12" s="118"/>
       <c r="AO12" s="118"/>
     </row>
-    <row r="13" spans="1:46" ht="17">
+    <row r="13" spans="1:46" ht="18.399999999999999">
       <c r="E13" s="129" t="s">
         <v>179</v>
       </c>
@@ -4721,7 +4728,7 @@
       <c r="AN13" s="118"/>
       <c r="AO13" s="118"/>
     </row>
-    <row r="14" spans="1:46" ht="17">
+    <row r="14" spans="1:46" ht="18">
       <c r="D14" t="s">
         <v>181</v>
       </c>
@@ -4738,7 +4745,7 @@
       <c r="AD14" s="58"/>
       <c r="AF14" s="58"/>
     </row>
-    <row r="15" spans="1:46" ht="17">
+    <row r="15" spans="1:46" ht="18">
       <c r="D15" t="s">
         <v>182</v>
       </c>
@@ -4755,7 +4762,7 @@
       <c r="AD15" s="58"/>
       <c r="AF15" s="58"/>
     </row>
-    <row r="16" spans="1:46" ht="17">
+    <row r="16" spans="1:46" ht="18">
       <c r="D16" s="132" t="s">
         <v>183</v>
       </c>
@@ -4773,7 +4780,7 @@
       <c r="AD16" s="84"/>
       <c r="AF16" s="84"/>
     </row>
-    <row r="17" spans="4:40" ht="17">
+    <row r="17" spans="4:40" ht="18">
       <c r="D17" t="s">
         <v>184</v>
       </c>
@@ -4791,7 +4798,7 @@
       <c r="AD17" s="84"/>
       <c r="AF17" s="84"/>
     </row>
-    <row r="18" spans="4:40" ht="17">
+    <row r="18" spans="4:40" ht="18">
       <c r="D18" t="s">
         <v>185</v>
       </c>
@@ -4810,7 +4817,7 @@
       <c r="E19" s="130"/>
       <c r="F19" s="105"/>
     </row>
-    <row r="20" spans="4:40" ht="15">
+    <row r="20" spans="4:40" ht="15.75">
       <c r="D20" t="s">
         <v>187</v>
       </c>
@@ -4853,7 +4860,7 @@
       <c r="E25" s="131"/>
       <c r="F25" s="123"/>
     </row>
-    <row r="26" spans="4:40">
+    <row r="26" spans="4:40" ht="12.75">
       <c r="D26" t="s">
         <v>193</v>
       </c>

</xml_diff>